<commit_message>
Ruta para consulta dep desde el bot
</commit_message>
<xml_diff>
--- a/src/public/uploads/BVCC.xlsx
+++ b/src/public/uploads/BVCC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliocesarmendoza/Desktop/pipApp/Backend-pi/src/public/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2EA63C6-5665-2945-9279-4D9E44358F97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89EB0C1-DCD8-3C40-89CB-B62C2940DFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64000" yWindow="11880" windowWidth="19120" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="5020" windowWidth="38400" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BarrioVereda" sheetId="1" r:id="rId1"/>
@@ -2473,10 +2473,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:C331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B200" sqref="B200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6140,6 +6141,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3D5556-04C1-0544-8C5E-2F0BAC19289E}">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:D331"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>